<commit_message>
loading into pyomo works 2
</commit_message>
<xml_diff>
--- a/excel files/play.xlsx
+++ b/excel files/play.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF67C162-F5D5-4065-B796-D49B2671B603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3A0C68-6D3F-4ED1-9BCD-467C439E5469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="2" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Intervals" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
   <si>
     <t>components</t>
   </si>
@@ -133,9 +133,6 @@
     <t>equations</t>
   </si>
   <si>
-    <t>prop</t>
-  </si>
-  <si>
     <t>conversion_factor</t>
   </si>
   <si>
@@ -145,18 +142,12 @@
     <t>inputs</t>
   </si>
   <si>
-    <t>ace,prop</t>
-  </si>
-  <si>
     <t>has_seperation</t>
   </si>
   <si>
     <t>seperation_coef</t>
   </si>
   <si>
-    <t>sep1</t>
-  </si>
-  <si>
     <t>sep2</t>
   </si>
   <si>
@@ -178,44 +169,59 @@
     <t>ace == 0.117 * glu, prop == 0.3243* glu</t>
   </si>
   <si>
-    <t>[0.8,0.2];[0.2,0.8]</t>
-  </si>
-  <si>
     <t xml:space="preserve">plastic </t>
   </si>
   <si>
-    <t>other_input</t>
-  </si>
-  <si>
-    <t>xyl</t>
-  </si>
-  <si>
     <t>phb</t>
   </si>
   <si>
-    <t>ace, prop</t>
-  </si>
-  <si>
     <t>phb == 0.22 *prop + 0.1 *ace</t>
   </si>
   <si>
     <t>prop == 0.3243* xyl</t>
   </si>
   <si>
-    <t>waste</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
     <t xml:space="preserve">phb </t>
+  </si>
+  <si>
+    <t>input_bounds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gold </t>
+  </si>
+  <si>
+    <t>silver</t>
+  </si>
+  <si>
+    <t>sep1; split1</t>
+  </si>
+  <si>
+    <t>sep1;split2</t>
+  </si>
+  <si>
+    <t>ag</t>
+  </si>
+  <si>
+    <t>au</t>
+  </si>
+  <si>
+    <t>ace,lac,au</t>
+  </si>
+  <si>
+    <t>lac,ace</t>
+  </si>
+  <si>
+    <t>[0,1];[0.2,0.8]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,8 +235,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,24 +252,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -393,22 +394,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -426,13 +416,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -440,47 +427,43 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -530,13 +513,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>768350</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -629,7 +612,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>755650</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -716,13 +699,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>11546</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>86591</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>1229591</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>92364</xdr:rowOff>
@@ -822,13 +805,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>65811</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>83127</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1194955</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -1442,25 +1425,25 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1486,12 +1469,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" s="12">
         <v>20</v>
@@ -1512,157 +1495,157 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="16">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="24">
+        <v>0</v>
+      </c>
+      <c r="D3" s="24">
+        <v>100</v>
+      </c>
+      <c r="E3" s="24">
+        <v>0</v>
+      </c>
+      <c r="F3" s="24">
+        <v>0</v>
+      </c>
+      <c r="G3" s="24">
+        <v>0</v>
+      </c>
+      <c r="H3" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="24">
+        <v>0</v>
+      </c>
+      <c r="D4" s="24">
+        <v>100</v>
+      </c>
+      <c r="E4" s="24">
+        <v>0</v>
+      </c>
+      <c r="F4" s="24">
+        <v>0</v>
+      </c>
+      <c r="G4" s="24">
+        <v>0</v>
+      </c>
+      <c r="H4" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="16">
+        <v>3</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="24">
+        <v>0</v>
+      </c>
+      <c r="D5" s="24">
+        <v>100</v>
+      </c>
+      <c r="E5" s="24">
+        <v>0</v>
+      </c>
+      <c r="F5" s="24">
+        <v>0</v>
+      </c>
+      <c r="G5" s="24">
+        <v>0</v>
+      </c>
+      <c r="H5" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="12">
+        <v>0</v>
+      </c>
+      <c r="F6" s="12">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="G6" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="12">
-        <v>20</v>
-      </c>
-      <c r="D3" s="12">
-        <v>100</v>
-      </c>
-      <c r="E3" s="12">
-        <v>1.2</v>
-      </c>
-      <c r="F3" s="12">
-        <v>0</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" s="12">
+      <c r="H6" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="17">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="27">
+        <v>3</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="12">
+        <v>0</v>
+      </c>
+      <c r="F7" s="12">
         <v>2</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="30">
-        <v>0</v>
-      </c>
-      <c r="D4" s="30">
-        <v>100</v>
-      </c>
-      <c r="E4" s="30">
-        <v>0</v>
-      </c>
-      <c r="F4" s="30">
-        <v>0</v>
-      </c>
-      <c r="G4" s="30">
-        <v>0</v>
-      </c>
-      <c r="H4" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="17">
-        <v>3</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="30">
-        <v>0</v>
-      </c>
-      <c r="D5" s="30">
-        <v>100</v>
-      </c>
-      <c r="E5" s="30">
-        <v>0</v>
-      </c>
-      <c r="F5" s="30">
-        <v>0</v>
-      </c>
-      <c r="G5" s="30">
-        <v>0</v>
-      </c>
-      <c r="H5" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="17">
-        <v>3</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="30">
-        <v>0</v>
-      </c>
-      <c r="D6" s="30">
-        <v>100</v>
-      </c>
-      <c r="E6" s="30">
-        <v>0</v>
-      </c>
-      <c r="F6" s="30">
-        <v>0</v>
-      </c>
-      <c r="G6" s="30">
-        <v>0</v>
-      </c>
-      <c r="H6" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="12">
-        <v>0</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="12">
-        <v>0</v>
-      </c>
-      <c r="F7" s="12">
-        <v>1</v>
-      </c>
       <c r="G7" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H7" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="17">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="27">
         <v>3</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>54</v>
+      <c r="B8" s="27" t="s">
+        <v>50</v>
       </c>
       <c r="C8" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="12">
+        <v>0</v>
+      </c>
+      <c r="F8" s="12">
+        <v>3</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>55</v>
-      </c>
-      <c r="E8" s="12">
-        <v>0</v>
-      </c>
-      <c r="F8" s="12">
-        <v>1</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>50</v>
       </c>
       <c r="H8" s="12">
         <v>1</v>
@@ -1670,8 +1653,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="E13:G13 E2:F9 H2:H9">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="E12:G12 E2:F8 H2:H8">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1683,29 +1666,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2DC50F-7E38-4E45-9660-C41E1DA6142A}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.08984375" customWidth="1"/>
-    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.26953125" customWidth="1"/>
-    <col min="10" max="10" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1713,153 +1697,162 @@
         <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N1" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
-        <v>35</v>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2">
+        <v>0.26675654674413302</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3">
+        <v>0.28253562825913597</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="12">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" t="s">
         <v>45</v>
       </c>
-      <c r="F2">
-        <v>0.26675654674413302</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3">
-        <v>0.28253562825913597</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3" s="12">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.26792861197630802</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
       <c r="H4">
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="12">
         <v>0</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
@@ -1868,24 +1861,33 @@
       <c r="M4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="K5" s="12"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="K6" s="12"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="F7" s="11"/>
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D7" s="26"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="12"/>
       <c r="I7" s="12"/>
-      <c r="K7" s="12"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="C12 C13:D13 E12 E10 J8:J11 H8:I12">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="C12:C13 F12 F10 H8:H11 M8:N12 E13">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:D13">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1898,296 +1900,298 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9730D4B9-BF36-445D-9853-EF3DA446843F}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="13" max="13" width="8.81640625" customWidth="1"/>
+    <col min="13" max="13" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="E1" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="F1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" t="s">
-        <v>47</v>
+      <c r="G1" s="16" t="s">
+        <v>51</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="22">
+        <v>0</v>
+      </c>
+      <c r="C2" s="22">
+        <v>1</v>
+      </c>
+      <c r="D2" s="22">
+        <v>0</v>
+      </c>
+      <c r="E2" s="22">
+        <v>0</v>
+      </c>
+      <c r="F2" s="22">
+        <v>0</v>
+      </c>
+      <c r="G2" s="22">
+        <v>0</v>
+      </c>
+      <c r="H2" s="22">
+        <v>0</v>
+      </c>
+      <c r="I2" s="17"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="21">
+        <v>0</v>
+      </c>
+      <c r="C3" s="21">
+        <v>0</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="21">
+        <v>0</v>
+      </c>
+      <c r="G3" s="21">
+        <v>0</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="17"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="23">
-        <v>0</v>
-      </c>
-      <c r="C2" s="12">
-        <v>0</v>
-      </c>
-      <c r="D2" s="23">
+      <c r="B4" s="22">
+        <v>0</v>
+      </c>
+      <c r="C4" s="22">
+        <v>0</v>
+      </c>
+      <c r="D4" s="22">
+        <v>0</v>
+      </c>
+      <c r="E4" s="22">
+        <v>0</v>
+      </c>
+      <c r="F4" s="22">
         <v>1</v>
       </c>
-      <c r="E2" s="13">
-        <v>0</v>
-      </c>
-      <c r="F2" s="13">
-        <v>0</v>
-      </c>
-      <c r="G2" s="13">
-        <v>0</v>
-      </c>
-      <c r="H2" s="18">
-        <v>0</v>
-      </c>
-      <c r="I2" s="18"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="23">
-        <v>0</v>
-      </c>
-      <c r="C3" s="23">
-        <v>0</v>
-      </c>
-      <c r="D3" s="22">
-        <v>0</v>
-      </c>
-      <c r="E3" s="28">
+      <c r="G4" s="22">
+        <v>0</v>
+      </c>
+      <c r="H4" s="22">
+        <v>0</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="15"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="22">
+        <v>0</v>
+      </c>
+      <c r="C5" s="22">
+        <v>0</v>
+      </c>
+      <c r="D5" s="22">
+        <v>0</v>
+      </c>
+      <c r="E5" s="22">
+        <v>0</v>
+      </c>
+      <c r="F5" s="22">
+        <v>0</v>
+      </c>
+      <c r="G5" s="22">
         <v>1</v>
       </c>
-      <c r="F3" s="23">
-        <v>0</v>
-      </c>
-      <c r="G3" s="24">
-        <v>0</v>
-      </c>
-      <c r="H3" s="29">
-        <v>0</v>
-      </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="23">
-        <v>0</v>
-      </c>
-      <c r="C4" s="23">
-        <v>0</v>
-      </c>
-      <c r="D4" s="12">
-        <v>0</v>
-      </c>
-      <c r="E4" s="23">
-        <v>0</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="32">
-        <v>0</v>
-      </c>
-      <c r="H4" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="16"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="16"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="H5" s="22">
+        <v>0</v>
+      </c>
+      <c r="I5" s="15"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="15"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="23">
-        <v>0</v>
-      </c>
-      <c r="C5" s="23">
-        <v>0</v>
-      </c>
-      <c r="D5" s="23">
-        <v>0</v>
-      </c>
-      <c r="E5" s="23">
-        <v>0</v>
-      </c>
-      <c r="F5" s="23">
-        <v>1</v>
-      </c>
-      <c r="G5" s="24">
-        <v>0</v>
-      </c>
-      <c r="H5" s="29">
-        <v>0</v>
-      </c>
-      <c r="I5" s="16"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="16"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="23">
-        <v>0</v>
-      </c>
-      <c r="C6" s="23">
-        <v>0</v>
-      </c>
-      <c r="D6" s="23">
-        <v>0</v>
-      </c>
-      <c r="E6" s="23">
-        <v>0</v>
-      </c>
-      <c r="F6" s="23">
-        <v>0</v>
-      </c>
-      <c r="G6" s="25">
-        <v>1</v>
-      </c>
-      <c r="H6" s="18">
-        <v>0</v>
-      </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="16"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="26">
-        <v>0</v>
-      </c>
-      <c r="C7" s="26">
-        <v>0</v>
-      </c>
-      <c r="D7" s="26">
-        <v>0</v>
-      </c>
-      <c r="E7" s="26">
-        <v>0</v>
-      </c>
-      <c r="F7" s="26">
-        <v>0</v>
-      </c>
-      <c r="G7" s="27">
-        <v>0</v>
-      </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="16"/>
-    </row>
-    <row r="8" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="22">
+        <v>0</v>
+      </c>
+      <c r="C6" s="22">
+        <v>0</v>
+      </c>
+      <c r="D6" s="22">
+        <v>0</v>
+      </c>
+      <c r="E6" s="22">
+        <v>0</v>
+      </c>
+      <c r="F6" s="22">
+        <v>0</v>
+      </c>
+      <c r="G6" s="22">
+        <v>0</v>
+      </c>
+      <c r="H6" s="22">
+        <v>0</v>
+      </c>
+      <c r="I6" s="15"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="15"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="23">
+        <v>0</v>
+      </c>
+      <c r="C7" s="23">
+        <v>0</v>
+      </c>
+      <c r="D7" s="23">
+        <v>0</v>
+      </c>
+      <c r="E7" s="23">
+        <v>0</v>
+      </c>
+      <c r="F7" s="23">
+        <v>0</v>
+      </c>
+      <c r="G7" s="23">
+        <v>0</v>
+      </c>
+      <c r="H7" s="23">
+        <v>0</v>
+      </c>
+      <c r="I7" s="15"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="15"/>
+    </row>
+    <row r="8" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="18">
-        <v>0</v>
-      </c>
-      <c r="C8" s="29">
-        <v>0</v>
-      </c>
-      <c r="D8" s="22">
-        <v>0</v>
-      </c>
-      <c r="E8" s="29">
-        <v>0</v>
-      </c>
-      <c r="F8" s="18">
-        <v>0</v>
-      </c>
-      <c r="G8" s="29">
-        <v>0</v>
-      </c>
-      <c r="H8" s="18">
-        <v>0</v>
-      </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="16"/>
-    </row>
-    <row r="9" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-    </row>
-    <row r="10" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-    </row>
-    <row r="11" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-    </row>
-    <row r="12" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-    </row>
-    <row r="13" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.35"/>
+        <v>50</v>
+      </c>
+      <c r="B8" s="21">
+        <v>0</v>
+      </c>
+      <c r="C8" s="21">
+        <v>0</v>
+      </c>
+      <c r="D8" s="21">
+        <v>0</v>
+      </c>
+      <c r="E8" s="21">
+        <v>0</v>
+      </c>
+      <c r="F8" s="21">
+        <v>0</v>
+      </c>
+      <c r="G8" s="21">
+        <v>0</v>
+      </c>
+      <c r="H8" s="21">
+        <v>0</v>
+      </c>
+      <c r="I8" s="15"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="15"/>
+    </row>
+    <row r="9" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+    </row>
+    <row r="10" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+    </row>
+    <row r="11" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+    </row>
+    <row r="12" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+    </row>
+    <row r="13" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B14:H16 I16">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2197,7 +2201,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:J15">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2206,13 +2210,33 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:C4 B3:D3 B2 D2:M2 F3:M3 B5:M13 E4:M4">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="B9:M13 I2:M8 B2:H3 B5:H8">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:H4">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:H8">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -2230,18 +2254,18 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2267,7 +2291,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2293,7 +2317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -2319,7 +2343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2345,7 +2369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2390,24 +2414,24 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="5"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
@@ -2415,7 +2439,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
@@ -2423,7 +2447,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
@@ -2431,37 +2455,37 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="7"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="9"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>19</v>
       </c>
@@ -2469,7 +2493,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
@@ -2477,7 +2501,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>16</v>
       </c>

</xml_diff>